<commit_message>
Chatbot for procurement updated
</commit_message>
<xml_diff>
--- a/sample_data/03 JULY 2023 TATA (1).xlsx
+++ b/sample_data/03 JULY 2023 TATA (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6790"/>
+    <workbookView windowWidth="18350" windowHeight="6830"/>
   </bookViews>
   <sheets>
     <sheet name="export - 2023-07-03T092619.558" sheetId="1" r:id="rId1"/>
@@ -256,21 +256,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,65 +720,65 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1114,8 +1107,8 @@
   <sheetPr/>
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>

</xml_diff>